<commit_message>
code review - commit
</commit_message>
<xml_diff>
--- a/GPO Roster Avendra_Performer/Data/Config.xlsx
+++ b/GPO Roster Avendra_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubSai\GPO-Roster-Avendra\GPO Roster Avendra_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915E86D1-661A-4D44-90F1-9EB92CA97BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6272E4A-D36B-4F64-A120-FFB6A4E9D46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -294,7 +294,7 @@
     <t>SH</t>
   </si>
   <si>
-    <t>Dev</t>
+    <t>UAT</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3035,7 +3035,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>